<commit_message>
add new slots to Data, update version number, update data objects
</commit_message>
<xml_diff>
--- a/inst/Data.xlsx
+++ b/inst/Data.xlsx
@@ -1,581 +1,599 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\DLMtool\inst\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13130" windowHeight="6110"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Description" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Description" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abundance index</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recruitment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duration t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average catch over time t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depletion over time t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FMSY/M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BMSY/B0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Length at 50% maturity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Length at 95% maturity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean length Lc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modal length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Length at first capture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Length at full selection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current stock depletion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current stock abundance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current spawning stock abundance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Von Bertalanffy K parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Von Bertalanffy Linf parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Von Bertalanffy t0 parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV of length-at-age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Length-weight parameter a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Length-weight parameter b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steepness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Catch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Depletion over time t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Average catch over time t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Abundance index</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV FMSY/M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV BMSY/B0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV current stock depletion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV current stock abundance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV von B. K parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV von B. Linf parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV von B. t0 parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Length at 50% maturity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Length at first capture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Length at full selection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Length-weight parameter a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Length-weight parameter b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Steepness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sigma length composition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAL_bins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference OFL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference OFL type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cref</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iref</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bref</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Cref</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Iref</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Bref</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Rec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MPrec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MPeff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LHYear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nareas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Object</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The name of the Data object. Single value. Character string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Years that corresponding to catch and relative abundance data. Vector nyears long. Positive integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total annual catches. Matrix of nsim rows and nyears columns. Non-negative real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relative abundance index. Matrix of nsim rows and nyears columns. Non-negative real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recent recruitment strength. Vector of length nsim. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of years corresponding to AvC and Dt. Single value. Positive integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AvC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average catch over time t. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depletion over time t SSB(now)/SSB(now-t+1). Vector nsim long. Fraction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mort</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natural mortality rate. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FMSY_M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An assumed ratio of FMSY to M. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BMSY_B0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The most productive stock size relative to unfished. Vector nsim long. Fraction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Length at 50 percent maturity. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Length at 95 percent maturity. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean length time series. Matrix of nsim rows and nyears columns. Non-negative real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lbar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean length of catches over Lc. Matrix of nsim rows and nyears columns. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modal length of catches. Matrix of nsim rows and nyears columns. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Length at first capture. Matrix of nsim rows and nyears columns. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LFS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shortest length at full selection. Matrix of nsim rows and nyears columns. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catch at Age data. Array of dimensions nsim x nyears x MaxAge. Non-negative integers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stock depletion SSB(current)/SSB(unfished). Vector nsim long. Fraction.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An estimate of absolute current vulnerable abundance. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SpAbun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An estimate of absolute current spawning stock abundance. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vbK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The von Bertalanffy growth coefficient K. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vbLinf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum length. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vbt0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Theoretical age at length zero. Vector nsim long. Non-positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LenCV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation of length-at-age (assumed constant for all age classes). Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight-Length parameter alpha. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wlb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight-Length parameter beta. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">steep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steepness of stock-recruitment relationship. Vector nsim long. Value in the range of one-fifth to 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_Cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in annual catches. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_Dt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in depletion over time t. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_AvC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in average catches over time t. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_Ind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in the relative abundance index. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_Mort</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in natural mortality rate. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_FMSY_M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in the ratio in FMSY/M. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_BMSY_B0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in the position of the most productive stock size relative to unfished. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_Dep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in current stock depletion. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_Abun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in estimate of absolute current stock size. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_vbK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in the von Bertalanffy K parameter. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_vbLinf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in maximum length. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_vbt0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in age at length zero. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_L50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in length at 50 per cent maturity. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_LFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in length at first capture. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_LFS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in length at full selection. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_wla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in weight-length parameter a. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_wlb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in weight-length parameter b. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_steep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient of variation in steepness. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sigmaL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assumed observaton error of the length composition data. Vector nsim long. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxAge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum age. Vector nsim long. Positive integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The values delimiting the length bins for the catch-at-length data. Vector. Non-negative real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catch-at-length data. An array with dimensions nsim x nyears x length(CAL_bins). Non-negative integers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Units of the catch/absolute abundance estimates. Single value. Character string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ref</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A reference management level (eg a catch limit). Single value. Positive real number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ref_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of reference management level (eg 2009 catch limit). Single value. Character string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference or target catch level (eg MSY). Vector of length nsim. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference or target relative abundance index level (eg BMSY / B0). Vector of length nsim. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference or target biomass level (eg BMSY). Vector of length nsim. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_Cref</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Log-normal CV for reference or target catch level. Vector of length nsim. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_Iref</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Log-normalCV for reference or target relative abundance index level. Vector of length nsim. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_Bref</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Log-normal CV for reference or target biomass level. Vector of length nsim. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV_Rec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Log-normal CV for recent recruitment strength. Vector of length nsim. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The previous recommendation of a management procedure. Vector of length nsim. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The current level of effort. Vector of length nsim. Positive real numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The last historical year of the simulation (before projection). Single value. Positive integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of fishing areas. Vector of length nsim. Non-negative integer</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="189">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Catch</t>
+  </si>
+  <si>
+    <t>Abundance index</t>
+  </si>
+  <si>
+    <t>Recruitment</t>
+  </si>
+  <si>
+    <t>Duration t</t>
+  </si>
+  <si>
+    <t>Average catch over time t</t>
+  </si>
+  <si>
+    <t>Depletion over time t</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>FMSY/M</t>
+  </si>
+  <si>
+    <t>BMSY/B0</t>
+  </si>
+  <si>
+    <t>Length at 50% maturity</t>
+  </si>
+  <si>
+    <t>Length at 95% maturity</t>
+  </si>
+  <si>
+    <t>Mean length</t>
+  </si>
+  <si>
+    <t>Mean length Lc</t>
+  </si>
+  <si>
+    <t>Modal length</t>
+  </si>
+  <si>
+    <t>Length at first capture</t>
+  </si>
+  <si>
+    <t>Length at full selection</t>
+  </si>
+  <si>
+    <t>CAA</t>
+  </si>
+  <si>
+    <t>Current stock depletion</t>
+  </si>
+  <si>
+    <t>Current stock abundance</t>
+  </si>
+  <si>
+    <t>Current spawning stock abundance</t>
+  </si>
+  <si>
+    <t>Von Bertalanffy K parameter</t>
+  </si>
+  <si>
+    <t>Von Bertalanffy Linf parameter</t>
+  </si>
+  <si>
+    <t>Von Bertalanffy t0 parameter</t>
+  </si>
+  <si>
+    <t>CV of length-at-age</t>
+  </si>
+  <si>
+    <t>Length-weight parameter a</t>
+  </si>
+  <si>
+    <t>Length-weight parameter b</t>
+  </si>
+  <si>
+    <t>Steepness</t>
+  </si>
+  <si>
+    <t>CV Catch</t>
+  </si>
+  <si>
+    <t>CV Depletion over time t</t>
+  </si>
+  <si>
+    <t>CV Average catch over time t</t>
+  </si>
+  <si>
+    <t>CV Abundance index</t>
+  </si>
+  <si>
+    <t>CV M</t>
+  </si>
+  <si>
+    <t>CV FMSY/M</t>
+  </si>
+  <si>
+    <t>CV BMSY/B0</t>
+  </si>
+  <si>
+    <t>CV current stock depletion</t>
+  </si>
+  <si>
+    <t>CV current stock abundance</t>
+  </si>
+  <si>
+    <t>CV von B. K parameter</t>
+  </si>
+  <si>
+    <t>CV von B. Linf parameter</t>
+  </si>
+  <si>
+    <t>CV von B. t0 parameter</t>
+  </si>
+  <si>
+    <t>CV Length at 50% maturity</t>
+  </si>
+  <si>
+    <t>CV Length at first capture</t>
+  </si>
+  <si>
+    <t>CV Length at full selection</t>
+  </si>
+  <si>
+    <t>CV Length-weight parameter a</t>
+  </si>
+  <si>
+    <t>CV Length-weight parameter b</t>
+  </si>
+  <si>
+    <t>CV Steepness</t>
+  </si>
+  <si>
+    <t>Sigma length composition</t>
+  </si>
+  <si>
+    <t>Maximum age</t>
+  </si>
+  <si>
+    <t>CAL_bins</t>
+  </si>
+  <si>
+    <t>CAL</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Reference OFL</t>
+  </si>
+  <si>
+    <t>Reference OFL type</t>
+  </si>
+  <si>
+    <t>Cref</t>
+  </si>
+  <si>
+    <t>Iref</t>
+  </si>
+  <si>
+    <t>Bref</t>
+  </si>
+  <si>
+    <t>CV Cref</t>
+  </si>
+  <si>
+    <t>CV Iref</t>
+  </si>
+  <si>
+    <t>CV Bref</t>
+  </si>
+  <si>
+    <t>CV Rec</t>
+  </si>
+  <si>
+    <t>MPrec</t>
+  </si>
+  <si>
+    <t>MPeff</t>
+  </si>
+  <si>
+    <t>LHYear</t>
+  </si>
+  <si>
+    <t>nareas</t>
+  </si>
+  <si>
+    <t>Data Object</t>
+  </si>
+  <si>
+    <t>Slot</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>The name of the Data object. Single value. Character string</t>
+  </si>
+  <si>
+    <t>Years that corresponding to catch and relative abundance data. Vector nyears long. Positive integer</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>Total annual catches. Matrix of nsim rows and nyears columns. Non-negative real numbers</t>
+  </si>
+  <si>
+    <t>Ind</t>
+  </si>
+  <si>
+    <t>Relative abundance index. Matrix of nsim rows and nyears columns. Non-negative real numbers</t>
+  </si>
+  <si>
+    <t>Rec</t>
+  </si>
+  <si>
+    <t>Recent recruitment strength. Vector of length nsim. Positive real numbers</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>The number of years corresponding to AvC and Dt. Single value. Positive integer</t>
+  </si>
+  <si>
+    <t>AvC</t>
+  </si>
+  <si>
+    <t>Average catch over time t. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>Dt</t>
+  </si>
+  <si>
+    <t>Depletion over time t SSB(now)/SSB(now-t+1). Vector nsim long. Fraction</t>
+  </si>
+  <si>
+    <t>Mort</t>
+  </si>
+  <si>
+    <t>Natural mortality rate. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>FMSY_M</t>
+  </si>
+  <si>
+    <t>An assumed ratio of FMSY to M. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>BMSY_B0</t>
+  </si>
+  <si>
+    <t>The most productive stock size relative to unfished. Vector nsim long. Fraction</t>
+  </si>
+  <si>
+    <t>L50</t>
+  </si>
+  <si>
+    <t>Length at 50 percent maturity. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>L95</t>
+  </si>
+  <si>
+    <t>Length at 95 percent maturity. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>Mean length time series. Matrix of nsim rows and nyears columns. Non-negative real numbers</t>
+  </si>
+  <si>
+    <t>Lbar</t>
+  </si>
+  <si>
+    <t>Mean length of catches over Lc. Matrix of nsim rows and nyears columns. Positive real numbers</t>
+  </si>
+  <si>
+    <t>Lc</t>
+  </si>
+  <si>
+    <t>Modal length of catches. Matrix of nsim rows and nyears columns. Positive real numbers</t>
+  </si>
+  <si>
+    <t>LFC</t>
+  </si>
+  <si>
+    <t>Length at first capture. Matrix of nsim rows and nyears columns. Positive real numbers</t>
+  </si>
+  <si>
+    <t>LFS</t>
+  </si>
+  <si>
+    <t>Shortest length at full selection. Matrix of nsim rows and nyears columns. Positive real numbers</t>
+  </si>
+  <si>
+    <t>Catch at Age data. Array of dimensions nsim x nyears x MaxAge. Non-negative integers</t>
+  </si>
+  <si>
+    <t>Dep</t>
+  </si>
+  <si>
+    <t>Stock depletion SSB(current)/SSB(unfished). Vector nsim long. Fraction.</t>
+  </si>
+  <si>
+    <t>Abun</t>
+  </si>
+  <si>
+    <t>An estimate of absolute current vulnerable abundance. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>SpAbun</t>
+  </si>
+  <si>
+    <t>An estimate of absolute current spawning stock abundance. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>vbK</t>
+  </si>
+  <si>
+    <t>The von Bertalanffy growth coefficient K. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>vbLinf</t>
+  </si>
+  <si>
+    <t>Maximum length. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>vbt0</t>
+  </si>
+  <si>
+    <t>Theoretical age at length zero. Vector nsim long. Non-positive real numbers</t>
+  </si>
+  <si>
+    <t>LenCV</t>
+  </si>
+  <si>
+    <t>Coefficient of variation of length-at-age (assumed constant for all age classes). Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>wla</t>
+  </si>
+  <si>
+    <t>Weight-Length parameter alpha. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>wlb</t>
+  </si>
+  <si>
+    <t>Weight-Length parameter beta. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>steep</t>
+  </si>
+  <si>
+    <t>Steepness of stock-recruitment relationship. Vector nsim long. Value in the range of one-fifth to 1</t>
+  </si>
+  <si>
+    <t>CV_Cat</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in annual catches. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_Dt</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in depletion over time t. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_AvC</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in average catches over time t. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_Ind</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in the relative abundance index. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_Mort</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in natural mortality rate. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_FMSY_M</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in the ratio in FMSY/M. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_BMSY_B0</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in the position of the most productive stock size relative to unfished. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_Dep</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in current stock depletion. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_Abun</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in estimate of absolute current stock size. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_vbK</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in the von Bertalanffy K parameter. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_vbLinf</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in maximum length. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_vbt0</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in age at length zero. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_L50</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in length at 50 per cent maturity. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_LFC</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in length at first capture. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_LFS</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in length at full selection. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_wla</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in weight-length parameter a. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_wlb</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in weight-length parameter b. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_steep</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in steepness. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>sigmaL</t>
+  </si>
+  <si>
+    <t>Assumed observaton error of the length composition data. Vector nsim long. Positive real numbers</t>
+  </si>
+  <si>
+    <t>MaxAge</t>
+  </si>
+  <si>
+    <t>Maximum age. Vector nsim long. Positive integer</t>
+  </si>
+  <si>
+    <t>The values delimiting the length bins for the catch-at-length data. Vector. Non-negative real numbers</t>
+  </si>
+  <si>
+    <t>Catch-at-length data. An array with dimensions nsim x nyears x length(CAL_bins). Non-negative integers</t>
+  </si>
+  <si>
+    <t>Units of the catch/absolute abundance estimates. Single value. Character string</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>A reference management level (eg a catch limit). Single value. Positive real number</t>
+  </si>
+  <si>
+    <t>Ref_type</t>
+  </si>
+  <si>
+    <t>Type of reference management level (eg 2009 catch limit). Single value. Character string</t>
+  </si>
+  <si>
+    <t>Reference or target catch level (eg MSY). Vector of length nsim. Positive real numbers</t>
+  </si>
+  <si>
+    <t>Reference or target relative abundance index level (eg BMSY / B0). Vector of length nsim. Positive real numbers</t>
+  </si>
+  <si>
+    <t>Reference or target biomass level (eg BMSY). Vector of length nsim. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_Cref</t>
+  </si>
+  <si>
+    <t>Log-normal CV for reference or target catch level. Vector of length nsim. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_Iref</t>
+  </si>
+  <si>
+    <t>Log-normalCV for reference or target relative abundance index level. Vector of length nsim. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_Bref</t>
+  </si>
+  <si>
+    <t>Log-normal CV for reference or target biomass level. Vector of length nsim. Positive real numbers</t>
+  </si>
+  <si>
+    <t>CV_Rec</t>
+  </si>
+  <si>
+    <t>Log-normal CV for recent recruitment strength. Vector of length nsim. Positive real numbers</t>
+  </si>
+  <si>
+    <t>The previous recommendation of a management procedure. Vector of length nsim. Positive real numbers</t>
+  </si>
+  <si>
+    <t>The current level of effort. Vector of length nsim. Positive real numbers</t>
+  </si>
+  <si>
+    <t>The last historical year of the simulation (before projection). Single value. Positive integer</t>
+  </si>
+  <si>
+    <t>Number of fishing areas. Vector of length nsim. Non-negative integer</t>
+  </si>
+  <si>
+    <t>Common Name</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>sigmaR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -611,6 +629,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -892,361 +919,383 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A69"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="9.15" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="32.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="10.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="32.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -1257,7 +1306,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1268,7 +1317,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1279,7 +1328,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1290,7 +1339,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1301,7 +1350,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1312,7 +1361,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1323,7 +1372,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1334,7 +1383,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1345,7 +1394,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1356,7 +1405,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1367,7 +1416,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1378,7 +1427,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1389,7 +1438,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1400,7 +1449,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1411,7 +1460,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1422,7 +1471,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1433,7 +1482,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1444,7 +1493,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1455,7 +1504,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1466,7 +1515,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1477,7 +1526,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1488,7 +1537,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1499,7 +1548,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1510,7 +1559,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1521,7 +1570,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1532,7 +1581,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1543,7 +1592,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1554,7 +1603,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1565,7 +1614,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1576,7 +1625,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1587,7 +1636,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1598,7 +1647,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1609,7 +1658,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1620,7 +1669,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1631,7 +1680,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1642,7 +1691,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1653,7 +1702,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1664,7 +1713,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1675,7 +1724,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1686,7 +1735,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1697,7 +1746,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1708,7 +1757,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1719,7 +1768,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1730,7 +1779,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1741,7 +1790,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1752,7 +1801,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1763,7 +1812,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1774,7 +1823,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1785,7 +1834,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1796,7 +1845,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1807,7 +1856,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1818,7 +1867,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1829,7 +1878,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1840,7 +1889,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1851,7 +1900,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1862,7 +1911,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1873,7 +1922,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1884,7 +1933,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1895,7 +1944,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1906,7 +1955,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1917,7 +1966,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1928,7 +1977,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1939,7 +1988,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1950,7 +1999,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -1961,7 +2010,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -1974,6 +2023,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>